<commit_message>
Update 20210420.MDI Tags and fields.xlsx
</commit_message>
<xml_diff>
--- a/tooling/20210420.MDI Tags and fields.xlsx
+++ b/tooling/20210420.MDI Tags and fields.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tony.masse\OneDrive - LogRhythm, Inc\Tony.Masse\Projets\20210331.EZ-Cloud on Legacy SIEM\EZ-Cloud\tooling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{914C68F9-D76E-4B8C-80E4-1B4B41021217}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{3A48BD5D-662C-4407-87ED-C99186B605F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="32040" xr2:uid="{0393503C-83F5-471D-900E-F1C45181E793}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0393503C-83F5-471D-900E-F1C45181E793}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="279">
   <si>
     <t>Object</t>
   </si>
@@ -566,9 +566,6 @@
     <t>Vendor Message ID</t>
   </si>
   <si>
-    <t>Specific vendor for the log used to describe a type of event.vmid</t>
-  </si>
-  <si>
     <t>Vendor Info</t>
   </si>
   <si>
@@ -870,6 +867,12 @@
   </si>
   <si>
     <t>Network Tab</t>
+  </si>
+  <si>
+    <t>Specific vendor for the log used to describe a type of event.</t>
+  </si>
+  <si>
+    <t>vmid</t>
   </si>
 </sst>
 </file>
@@ -1732,10 +1735,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E1" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1743,27 +1746,27 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>265</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D4" s="1" t="b">
         <v>1</v>
@@ -1909,7 +1912,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>25</v>
@@ -2149,10 +2152,10 @@
         <v>68</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5" t="str">
@@ -2202,7 +2205,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>75</v>
@@ -2372,7 +2375,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>103</v>
@@ -2392,13 +2395,16 @@
       <c r="A44" s="4" t="s">
         <v>104</v>
       </c>
+      <c r="B44" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="C44" s="1" t="s">
         <v>105</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="5" t="str">
         <f>IF(ISBLANK(A44),"        //",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(template,"LABEL_TAG",A44),"VALUE_TAG",C44),"DISABLE_TAG",IF(D44,"true","false")),"SEP_TAG",IF(E44,"true","false")),"DESC_TAG",SUBSTITUTE(B44,"'","\'")),", value: ''",""),", disable: false",""),", separator: false",""))</f>
-        <v xml:space="preserve">        { label: 'Bits in', value: 'bitsin', description: '' },</v>
+        <v xml:space="preserve">        { label: 'Bits in', value: 'bitsin', description: 'In the context of the Impacted Host.' },</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2406,12 +2412,15 @@
         <v>106</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>107</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5" t="str">
         <f>IF(ISBLANK(A45),"        //",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(template,"LABEL_TAG",A45),"VALUE_TAG",C45),"DISABLE_TAG",IF(D45,"true","false")),"SEP_TAG",IF(E45,"true","false")),"DESC_TAG",SUBSTITUTE(B45,"'","\'")),", value: ''",""),", disable: false",""),", separator: false",""))</f>
-        <v xml:space="preserve">        { label: 'Bits out', description: 'bitsout' },</v>
+        <v xml:space="preserve">        { label: 'Bits out', value: 'bitsout', description: 'In the context of the Impacted Host.' },</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -3016,7 +3025,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D84" s="1" t="b">
         <v>1</v>
@@ -3050,23 +3059,26 @@
         <v>175</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>176</v>
+        <v>277</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>278</v>
       </c>
       <c r="E86" s="5"/>
       <c r="F86" s="5" t="str">
         <f>IF(ISBLANK(A86),"        //",SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(template,"LABEL_TAG",A86),"VALUE_TAG",C86),"DISABLE_TAG",IF(D86,"true","false")),"SEP_TAG",IF(E86,"true","false")),"DESC_TAG",SUBSTITUTE(B86,"'","\'")),", value: ''",""),", disable: false",""),", separator: false",""))</f>
-        <v xml:space="preserve">        { label: 'Vendor Message ID', description: 'Specific vendor for the log used to describe a type of event.vmid' },</v>
+        <v xml:space="preserve">        { label: 'Vendor Message ID', value: 'vmid', description: 'Specific vendor for the log used to describe a type of event.' },</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="C87" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="E87" s="5"/>
       <c r="F87" s="5" t="str">
@@ -3076,13 +3088,13 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="C88" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="E88" s="5"/>
       <c r="F88" s="5" t="str">
@@ -3092,13 +3104,13 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="C89" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="E89" s="5"/>
       <c r="F89" s="5" t="str">
@@ -3108,13 +3120,13 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="C90" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E90" s="5"/>
       <c r="F90" s="5" t="str">
@@ -3132,7 +3144,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D92" s="1" t="b">
         <v>1</v>
@@ -3147,13 +3159,13 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="C93" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="E93" s="5"/>
       <c r="F93" s="5" t="str">
@@ -3163,13 +3175,13 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="C94" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>194</v>
       </c>
       <c r="E94" s="5"/>
       <c r="F94" s="5" t="str">
@@ -3179,13 +3191,13 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="C95" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="E95" s="5"/>
       <c r="F95" s="5" t="str">
@@ -3195,13 +3207,13 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="C96" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="E96" s="5"/>
       <c r="F96" s="5" t="str">
@@ -3211,13 +3223,13 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="C97" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="E97" s="5"/>
       <c r="F97" s="5" t="str">
@@ -3227,13 +3239,13 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="C98" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="E98" s="5"/>
       <c r="F98" s="5" t="str">
@@ -3243,13 +3255,13 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="C99" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="E99" s="5"/>
       <c r="F99" s="5" t="str">
@@ -3259,13 +3271,13 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="C100" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="E100" s="5"/>
       <c r="F100" s="5" t="str">
@@ -3275,13 +3287,13 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="C101" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>215</v>
       </c>
       <c r="E101" s="5"/>
       <c r="F101" s="5" t="str">
@@ -3291,13 +3303,13 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="C102" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="E102" s="5"/>
       <c r="F102" s="5" t="str">
@@ -3307,13 +3319,13 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="C103" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="E103" s="5"/>
       <c r="F103" s="5" t="str">
@@ -3331,7 +3343,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D105" s="1" t="b">
         <v>1</v>
@@ -3346,13 +3358,13 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B106" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="C106" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>224</v>
       </c>
       <c r="E106" s="5"/>
       <c r="F106" s="5" t="str">
@@ -3362,13 +3374,13 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="C107" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="E107" s="5"/>
       <c r="F107" s="5" t="str">
@@ -3378,13 +3390,13 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B108" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="C108" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="E108" s="5"/>
       <c r="F108" s="5" t="str">
@@ -3394,13 +3406,13 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="C109" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>233</v>
       </c>
       <c r="E109" s="5"/>
       <c r="F109" s="5" t="str">
@@ -3410,13 +3422,13 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B110" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="C110" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="E110" s="5"/>
       <c r="F110" s="5" t="str">
@@ -3434,7 +3446,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D112" s="1" t="b">
         <v>1</v>
@@ -3449,13 +3461,13 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B113" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="C113" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="E113" s="5"/>
       <c r="F113" s="5" t="str">
@@ -3465,13 +3477,13 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="C114" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>242</v>
       </c>
       <c r="E114" s="5"/>
       <c r="F114" s="5" t="str">
@@ -3481,13 +3493,13 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="C115" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>245</v>
       </c>
       <c r="E115" s="5"/>
       <c r="F115" s="5" t="str">
@@ -3497,13 +3509,13 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B116" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>247</v>
       </c>
       <c r="E116" s="5"/>
       <c r="F116" s="5" t="str">
@@ -3513,13 +3525,13 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B117" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="C117" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="E117" s="5"/>
       <c r="F117" s="5" t="str">
@@ -3529,13 +3541,13 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B118" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="C118" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="E118" s="5"/>
       <c r="F118" s="5" t="str">
@@ -3545,13 +3557,13 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B119" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="C119" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>256</v>
       </c>
       <c r="E119" s="5"/>
       <c r="F119" s="5" t="str">
@@ -3561,13 +3573,13 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="B120" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="B120" s="10" t="s">
+      <c r="C120" s="10" t="s">
         <v>258</v>
-      </c>
-      <c r="C120" s="10" t="s">
-        <v>259</v>
       </c>
       <c r="D120" s="10"/>
       <c r="E120" s="11"/>

</xml_diff>